<commit_message>
Feat: Email scraper now logs errors in log file
</commit_message>
<xml_diff>
--- a/email_scripts/order.xlsx
+++ b/email_scripts/order.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,14 +483,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="10.8"/>
-    <col customWidth="1" max="2" min="2" width="24"/>
+    <col customWidth="1" max="2" min="2" width="36"/>
     <col customWidth="1" max="3" min="3" width="4.8"/>
     <col customWidth="1" max="4" min="4" width="9.6"/>
     <col customWidth="1" max="5" min="5" width="4.8"/>
     <col customWidth="1" max="6" min="6" width="10.8"/>
-    <col customWidth="1" max="7" min="7" width="24"/>
+    <col customWidth="1" max="7" min="7" width="36"/>
     <col customWidth="1" max="8" min="8" width="4.8"/>
-    <col customWidth="1" max="9" min="9" width="4.8"/>
+    <col customWidth="1" max="9" min="9" width="9.6"/>
     <col customWidth="1" max="10" min="10" width="4.8"/>
   </cols>
   <sheetData>
@@ -584,14 +584,23 @@
       <c r="C3" s="6" t="n"/>
       <c r="D3" s="6" t="n"/>
       <c r="E3" s="6" t="n"/>
+      <c r="F3" s="6" t="n"/>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>XL LAYS</t>
+        </is>
+      </c>
+      <c r="H3" s="6" t="n"/>
+      <c r="I3" s="6" t="n"/>
+      <c r="J3" s="6" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>DORITOS NACHO CHEESE</t>
+          <t>DORITOS COOL RANCH</t>
         </is>
       </c>
       <c r="C4" s="10" t="n">
@@ -599,55 +608,293 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>FL-64203</t>
+          <t>FL-64132</t>
         </is>
       </c>
       <c r="E4" s="10" t="n">
         <v>7</v>
       </c>
+      <c r="F4" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>XL LAYS SOUR CREAM &amp; ONION</t>
+        </is>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="I4" s="8" t="inlineStr">
+        <is>
+          <t>FL-19963</t>
+        </is>
+      </c>
+      <c r="J4" s="10" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n"/>
-      <c r="B5" s="11" t="n"/>
-      <c r="C5" s="11" t="n"/>
-      <c r="D5" s="11" t="n"/>
-      <c r="E5" s="11" t="n"/>
+      <c r="A5" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>DORITOS TACO</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
+        <is>
+          <t>FL-64191</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
+        <is>
+          <t>XL WAVY LAYS BBQ</t>
+        </is>
+      </c>
+      <c r="H5" s="10" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>FL-04349</t>
+        </is>
+      </c>
+      <c r="J5" s="10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>DORITOS SPICY NACHO</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>FL-64204</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" s="11" t="n"/>
+      <c r="G6" s="11" t="n"/>
+      <c r="H6" s="11" t="n"/>
+      <c r="I6" s="11" t="n"/>
+      <c r="J6" s="11" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>DORITOS JACKED RANCH HOT WINGS</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>FL-64226</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" s="6" t="n"/>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>BAKED - REDUCED FAT</t>
+        </is>
+      </c>
+      <c r="H7" s="6" t="n"/>
+      <c r="I7" s="6" t="n"/>
+      <c r="J7" s="6" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="11" t="n"/>
+      <c r="B8" s="11" t="n"/>
+      <c r="C8" s="11" t="n"/>
+      <c r="D8" s="11" t="n"/>
+      <c r="E8" s="11" t="n"/>
+      <c r="F8" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>BAKED CHEETOS FLAMIN' HOT</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>FL-18391</t>
+        </is>
+      </c>
+      <c r="J8" s="10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>FRITOS</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="n"/>
+      <c r="D9" s="6" t="n"/>
+      <c r="E9" s="6" t="n"/>
+      <c r="F9" s="11" t="n"/>
+      <c r="G9" s="11" t="n"/>
+      <c r="H9" s="11" t="n"/>
+      <c r="I9" s="11" t="n"/>
+      <c r="J9" s="11" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>FRITOS SCOOPS</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="D10" s="8" t="inlineStr">
+        <is>
+          <t>FL-58932</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="inlineStr">
+        <is>
+          <t>FRITOS SPICY JALAPENO SCOOPS</t>
+        </is>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="D11" s="8" t="inlineStr">
+        <is>
+          <t>FL-15907</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n"/>
+      <c r="B12" s="11" t="n"/>
+      <c r="C12" s="11" t="n"/>
+      <c r="D12" s="11" t="n"/>
+      <c r="E12" s="11" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n"/>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>FAMILY SIZE LAYS</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="n"/>
+      <c r="D13" s="6" t="n"/>
+      <c r="E13" s="6" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>FS WAVY LAYS</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>FL-04389</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="n"/>
+      <c r="B15" s="11" t="n"/>
+      <c r="C15" s="11" t="n"/>
+      <c r="D15" s="11" t="n"/>
+      <c r="E15" s="11" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="12" t="inlineStr">
         <is>
           <t>NOTE:</t>
         </is>
       </c>
-      <c r="B7" s="13" t="n"/>
-      <c r="C7" s="13" t="n"/>
-      <c r="D7" s="13" t="n"/>
-      <c r="E7" s="13" t="n"/>
-      <c r="F7" s="13" t="n"/>
-      <c r="G7" s="13" t="n"/>
-      <c r="H7" s="13" t="n"/>
-      <c r="I7" s="13" t="n"/>
-      <c r="J7" s="13" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="14" t="inlineStr">
-        <is>
-          <t>Testing printing script</t>
-        </is>
-      </c>
-    </row>
-    <row r="9"/>
+      <c r="B17" s="13" t="n"/>
+      <c r="C17" s="13" t="n"/>
+      <c r="D17" s="13" t="n"/>
+      <c r="E17" s="13" t="n"/>
+      <c r="F17" s="13" t="n"/>
+      <c r="G17" s="13" t="n"/>
+      <c r="H17" s="13" t="n"/>
+      <c r="I17" s="13" t="n"/>
+      <c r="J17" s="13" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="14" t="inlineStr">
+        <is>
+          <t>Some notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A8:J9"/>
+    <mergeCell ref="A18:J19"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0" right="0" top="1"/>
   <pageSetup fitToHeight="0" fitToWidth="1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Arial"&amp;12 FRI&amp;C&amp;"Arial"&amp;14 CUSTOMER: West Freds&amp;R&amp;"Arial"&amp;10 DATE ORDER TAKEN: 2019-04-05</oddHeader>
-    <oddFooter>&amp;L&amp;"Arial"&amp;12 PULLED BY:____________&amp;C&amp;"Arial"&amp;12 FOR DELIVERY ON: SAT&amp;R&amp;"Arial"&amp;12 DELIVERED BY:____________</oddFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;12 FRI&amp;C&amp;"Arial"&amp;14 CUSTOMER: Test&amp;R&amp;"Arial"&amp;10 DATE ORDER TAKEN: 2019-04-19</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial"&amp;12 PULLED BY:____________&amp;C&amp;"Arial"&amp;12 FOR DELIVERY ON: FRI&amp;R&amp;"Arial"&amp;12 DELIVERED BY:____________</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>

</xml_diff>